<commit_message>
update 12/01 part 2
</commit_message>
<xml_diff>
--- a/Initialized_Data.xlsx
+++ b/Initialized_Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ef074c61d2afe73/Desktop/Stefano/In_the_NL/Thesis/Code/git_hub_repos/Thesis_main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_F25DC773A252ABDACC10484421DC4AE85BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{226A5402-69C0-4D34-98A0-477BEA137E9B}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="11_F25DC773A252ABDACC10484421DC4AE85BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F462AEB9-D509-486E-9E73-07EB54E681C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EV_data" sheetId="1" r:id="rId1"/>
-    <sheet name="time" sheetId="8" r:id="rId2"/>
+    <sheet name="demand" sheetId="8" r:id="rId2"/>
     <sheet name="EV_chargers" sheetId="7" r:id="rId3"/>
     <sheet name="grid_connection" sheetId="2" r:id="rId4"/>
     <sheet name="transformers" sheetId="3" r:id="rId5"/>
@@ -240,18 +240,6 @@
     <t>consumption_kwh_km</t>
   </si>
   <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>EV</t>
-  </si>
-  <si>
-    <t>electricity_demand</t>
-  </si>
-  <si>
-    <t>heating_demand</t>
-  </si>
-  <si>
     <t>Energy capacity [kWh]</t>
   </si>
   <si>
@@ -274,6 +262,18 @@
   </si>
   <si>
     <t>Max power [kW]</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Heating power demand [kW]</t>
+  </si>
+  <si>
+    <t>Electricity power demand [kW]</t>
+  </si>
+  <si>
+    <t>EV power demand [kW]</t>
   </si>
 </sst>
 </file>
@@ -637,22 +637,22 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>64</v>
@@ -716,148 +716,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3CEF5C-8F80-4D83-B766-BE0CCA7ADF11}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A75EA3B-87C0-4820-AD28-D888BE3A1108}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1029,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>